<commit_message>
tested exporting of edited documents, revised the database a bit
</commit_message>
<xml_diff>
--- a/implicaspection/report-templates/yorumkod-Bericht2_MitKommentaren.xlsx
+++ b/implicaspection/report-templates/yorumkod-Bericht2_MitKommentaren.xlsx
@@ -218,6 +218,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MP Taşıyıcı Ortam???</t>
         </r>
@@ -251,6 +252,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Mıknatıslama Tekniği???</t>
         </r>
@@ -284,6 +286,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">UV Işık Şiddeti???</t>
         </r>
@@ -317,6 +320,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Işık Mesafesi???</t>
         </r>
@@ -704,6 +708,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">???default???Muayene Bölgesi???KAYNAK+HAZ</t>
         </r>
@@ -1264,7 +1269,7 @@
             <family val="2"/>
             <charset val="162"/>
           </rPr>
-          <t xml:space="preserve">???is-emri-no???İş Emri No</t>
+          <t xml:space="preserve">???depend???İş Emri No???is-emri-no</t>
         </r>
       </text>
     </comment>
@@ -1278,7 +1283,7 @@
             <family val="2"/>
             <charset val="162"/>
           </rPr>
-          <t xml:space="preserve">???teklif-no??Teklif No</t>
+          <t xml:space="preserve">???depend???Teklif No???teklif-no</t>
         </r>
       </text>
     </comment>
@@ -3007,6 +3012,7 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3567,9 +3573,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>14040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>198360</xdr:rowOff>
+      <xdr:rowOff>198000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3582,8 +3588,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2277000" y="5213880"/>
-          <a:ext cx="1521360" cy="1079640"/>
+          <a:off x="2276280" y="5213880"/>
+          <a:ext cx="1521000" cy="1079280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3604,9 +3610,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>150480</xdr:colOff>
+      <xdr:colOff>150120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3620,7 +3626,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="74160" y="5230080"/>
-          <a:ext cx="1783080" cy="901800"/>
+          <a:ext cx="1782000" cy="901440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3643,7 +3649,7 @@
   <dimension ref="A1:AK74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+      <selection pane="topLeft" activeCell="AA7" activeCellId="0" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>